<commit_message>
Completed Spec Analysis and Main Figures!
</commit_message>
<xml_diff>
--- a/results/Tbl_Multinom2.xlsx
+++ b/results/Tbl_Multinom2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="112">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -340,6 +340,21 @@
   </si>
   <si>
     <t>Panel C. Model Statistics</t>
+  </si>
+  <si>
+    <t>Results: % Positive at CI95</t>
+  </si>
+  <si>
+    <t>Results: % Negative at CI95</t>
+  </si>
+  <si>
+    <t>-1.576 *</t>
+  </si>
+  <si>
+    <t>-11.120 **</t>
+  </si>
+  <si>
+    <t>-10.076 *</t>
   </si>
 </sst>
 </file>
@@ -864,7 +879,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -899,6 +914,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1220,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:H69"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1755,8 +1774,11 @@
       <c r="C28" s="1">
         <v>-1.5049999999999999</v>
       </c>
+      <c r="G28" s="1">
+        <v>-1.9750000000000001</v>
+      </c>
       <c r="H28" s="1">
-        <v>-1.9990000000000001</v>
+        <v>1.194</v>
       </c>
       <c r="K28" s="3"/>
     </row>
@@ -1767,8 +1789,11 @@
       <c r="D29" s="1">
         <v>-0.40799999999999997</v>
       </c>
+      <c r="G29" s="1">
+        <v>-0.113</v>
+      </c>
       <c r="H29" s="1">
-        <v>-0.34100000000000003</v>
+        <v>-1.2869999999999999</v>
       </c>
       <c r="K29" s="3"/>
     </row>
@@ -1779,8 +1804,11 @@
       <c r="E30" s="1">
         <v>-4.9139999999999997</v>
       </c>
+      <c r="G30" s="1">
+        <v>-11.859</v>
+      </c>
       <c r="H30" s="1">
-        <v>-6.0650000000000004</v>
+        <v>-7.5279999999999996</v>
       </c>
       <c r="K30" s="3"/>
     </row>
@@ -1791,40 +1819,37 @@
       <c r="F31" s="1">
         <v>-1.0880000000000001</v>
       </c>
-      <c r="H31" s="1">
-        <v>0.51500000000000001</v>
+      <c r="G31" s="1">
+        <v>2.0059999999999998</v>
       </c>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9">
-        <v>7.4889999999999999</v>
-      </c>
-      <c r="H32" s="9"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17">
+        <v>18.841999999999999</v>
+      </c>
+      <c r="H32" s="17"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="A33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>105</v>
+      <c r="A34" s="15" t="s">
+        <v>108</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1832,632 +1857,682 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
+      <c r="H34" s="9">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D37" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E37" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F37" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G37" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H37" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C38" s="1">
         <v>2.391</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D38" s="1">
         <v>4.8049999999999997</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E38" s="1">
         <v>1.4139999999999999</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F38" s="1">
         <v>2.2160000000000002</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G38" s="1">
         <v>1.9550000000000001</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H38" s="1">
         <v>4.2869999999999999</v>
       </c>
-      <c r="K36" s="3"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C40" s="1">
         <v>-1.024</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D40" s="1">
         <v>-1.0669999999999999</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E40" s="1">
         <v>-0.439</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F40" s="1">
         <v>-0.99199999999999999</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G40" s="1">
         <v>-1.03</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H40" s="1">
         <v>-0.53500000000000003</v>
-      </c>
-      <c r="K38" s="3"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0.502</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0.155</v>
-      </c>
-      <c r="F39" s="1">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0.313</v>
-      </c>
-      <c r="H39" s="1">
-        <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="K39" s="3"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.502</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.155</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.313</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C43" s="1">
         <v>0.74099999999999999</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D43" s="1">
         <v>0.67700000000000005</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E43" s="1">
         <v>0.68700000000000006</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F43" s="1">
         <v>0.78100000000000003</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G43" s="1">
         <v>0.80800000000000005</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H43" s="1">
         <v>0.46100000000000002</v>
       </c>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1.202</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1.5660000000000001</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="F42" s="1">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="G42" s="1">
-        <v>1.454</v>
-      </c>
-      <c r="H42" s="1">
-        <v>1.331</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="K43" s="4"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.202</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1.454</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1.331</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="1">
-        <v>-0.84099999999999997</v>
-      </c>
-      <c r="D47" s="1">
-        <v>-1.516</v>
-      </c>
-      <c r="E47" s="1">
-        <v>-0.22800000000000001</v>
-      </c>
-      <c r="F47" s="1">
-        <v>-0.79900000000000004</v>
-      </c>
-      <c r="G47" s="1">
-        <v>-1.1080000000000001</v>
-      </c>
-      <c r="H47" s="1">
-        <v>-0.89300000000000002</v>
+        <v>83</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1.1679999999999999</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1.2310000000000001</v>
-      </c>
-      <c r="E48" s="1">
-        <v>1.3160000000000001</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1.208</v>
-      </c>
-      <c r="G48" s="1">
-        <v>1.0780000000000001</v>
-      </c>
-      <c r="H48" s="1">
-        <v>1.2490000000000001</v>
+      <c r="A48" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C49" s="1">
-        <v>1.254</v>
+        <v>-0.84099999999999997</v>
       </c>
       <c r="D49" s="1">
-        <v>1.7190000000000001</v>
+        <v>-1.516</v>
       </c>
       <c r="E49" s="1">
-        <v>1.4119999999999999</v>
+        <v>-0.22800000000000001</v>
       </c>
       <c r="F49" s="1">
-        <v>1.3069999999999999</v>
+        <v>-0.79900000000000004</v>
       </c>
       <c r="G49" s="1">
-        <v>1.2350000000000001</v>
+        <v>-1.1080000000000001</v>
       </c>
       <c r="H49" s="1">
-        <v>1.857</v>
+        <v>-0.89300000000000002</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C50" s="1">
-        <v>4.2080000000000002</v>
+        <v>1.1679999999999999</v>
       </c>
       <c r="D50" s="1">
-        <v>4.2850000000000001</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="E50" s="1">
-        <v>5.8419999999999996</v>
+        <v>1.3160000000000001</v>
       </c>
       <c r="F50" s="1">
-        <v>4.1719999999999997</v>
+        <v>1.208</v>
       </c>
       <c r="G50" s="1">
-        <v>4.016</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="H50" s="1">
-        <v>6.2350000000000003</v>
+        <v>1.2490000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C51" s="1">
-        <v>-3.19</v>
+        <v>1.254</v>
       </c>
       <c r="D51" s="1">
-        <v>-2.91</v>
+        <v>1.7190000000000001</v>
       </c>
       <c r="E51" s="1">
-        <v>-4.9740000000000002</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="F51" s="1">
-        <v>-3.1909999999999998</v>
+        <v>1.3069999999999999</v>
       </c>
       <c r="G51" s="1">
-        <v>-3.2050000000000001</v>
+        <v>1.2350000000000001</v>
       </c>
       <c r="H51" s="1">
-        <v>-5.0030000000000001</v>
+        <v>1.857</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>90</v>
+      <c r="A52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4.2080000000000002</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4.2850000000000001</v>
+      </c>
+      <c r="E52" s="1">
+        <v>5.8419999999999996</v>
+      </c>
+      <c r="F52" s="1">
+        <v>4.1719999999999997</v>
+      </c>
+      <c r="G52" s="1">
+        <v>4.016</v>
+      </c>
+      <c r="H52" s="1">
+        <v>6.2350000000000003</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C53" s="1">
-        <v>-0.183</v>
+        <v>-3.19</v>
       </c>
       <c r="D53" s="1">
-        <v>-3.3000000000000002E-2</v>
+        <v>-2.91</v>
       </c>
       <c r="E53" s="1">
-        <v>-0.128</v>
+        <v>-4.9740000000000002</v>
       </c>
       <c r="F53" s="1">
-        <v>-0.16300000000000001</v>
+        <v>-3.1909999999999998</v>
       </c>
       <c r="G53" s="1">
-        <v>-8.8999999999999996E-2</v>
+        <v>-3.2050000000000001</v>
       </c>
       <c r="H53" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>-5.0030000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="1">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="D54" s="1">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="F54" s="1">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="G54" s="1">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="H54" s="1">
-        <v>0.72299999999999998</v>
+      <c r="A54" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="1">
+        <v>-0.183</v>
+      </c>
+      <c r="D55" s="1">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="E55" s="1">
+        <v>-0.128</v>
+      </c>
+      <c r="F55" s="1">
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="G55" s="1">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="H55" s="1">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C59" s="1">
         <v>-0.26300000000000001</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D59" s="1">
         <v>-0.71799999999999997</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E59" s="1">
         <v>-0.32400000000000001</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F59" s="1">
         <v>-0.29199999999999998</v>
       </c>
-      <c r="G57" s="1">
+      <c r="G59" s="1">
         <v>-0.20200000000000001</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H59" s="1">
         <v>-0.80300000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="1">
-        <v>-5.2999999999999999E-2</v>
-      </c>
-      <c r="H59" s="1">
-        <v>6.8000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D60" s="1">
-        <v>-0.52600000000000002</v>
-      </c>
-      <c r="H60" s="1">
-        <v>-0.55600000000000005</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E61" s="1">
-        <v>-2.589</v>
+        <v>96</v>
+      </c>
+      <c r="C61" s="1">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.16700000000000001</v>
       </c>
       <c r="H61" s="1">
-        <v>-3.2440000000000002</v>
+        <v>3.536</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="1">
+        <v>-0.52600000000000002</v>
+      </c>
+      <c r="G62" s="1">
+        <v>-0.51400000000000001</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="1">
+        <v>-2.589</v>
+      </c>
+      <c r="G63" s="1">
+        <v>-3.4550000000000001</v>
+      </c>
+      <c r="H63" s="1">
+        <v>-4.157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F64" s="1">
         <v>-0.249</v>
       </c>
-      <c r="H62" s="1">
-        <v>0.89500000000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="G64" s="1">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G63" s="1">
-        <v>1.726</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="G65" s="1">
+        <v>2.339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B69" s="1">
         <v>88</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C69" s="1">
         <v>88</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D69" s="1">
         <v>88</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E69" s="1">
         <v>88</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F69" s="1">
         <v>88</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G69" s="1">
         <v>88</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H69" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B70" s="1">
         <v>0</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C70" s="1">
         <v>0.52200000000000002</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D70" s="1">
         <v>0.53600000000000003</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E70" s="1">
         <v>0.54400000000000004</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F70" s="1">
         <v>0.52100000000000002</v>
       </c>
-      <c r="G66" s="1">
-        <v>0.52100000000000002</v>
-      </c>
-      <c r="H66" s="1">
-        <v>0.57799999999999996</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="G70" s="1">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B71" s="1">
         <v>160.215</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C71" s="1">
         <v>109.63200000000001</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D71" s="1">
         <v>107.67400000000001</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E71" s="1">
         <v>106.587</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F71" s="1">
         <v>109.721</v>
       </c>
-      <c r="G67" s="1">
-        <v>109.664</v>
-      </c>
-      <c r="H67" s="1">
-        <v>101.94199999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14" t="s">
+      <c r="G71" s="1">
+        <v>98.929000000000002</v>
+      </c>
+      <c r="H71" s="1">
+        <v>70.667000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="14">
+      <c r="B72" s="14">
         <v>-80.106999999999999</v>
       </c>
-      <c r="C68" s="14">
+      <c r="C72" s="14">
         <v>-54.816000000000003</v>
       </c>
-      <c r="D68" s="14">
+      <c r="D72" s="14">
         <v>-53.837000000000003</v>
       </c>
-      <c r="E68" s="14">
+      <c r="E72" s="14">
         <v>-53.293999999999997</v>
       </c>
-      <c r="F68" s="14">
+      <c r="F72" s="14">
         <v>-54.86</v>
       </c>
-      <c r="G68" s="14">
-        <v>-54.832000000000001</v>
-      </c>
-      <c r="H68" s="14">
-        <v>-50.970999999999997</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="G72" s="14">
+        <v>-49.465000000000003</v>
+      </c>
+      <c r="H72" s="14">
+        <v>-35.334000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>